<commit_message>
Added present value of annuity sheet
</commit_message>
<xml_diff>
--- a/Time_value_of_Money/Present_Value.xlsx
+++ b/Time_value_of_Money/Present_Value.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devereweaver/Principles-of-Finance-with-Excel/Time_value_of_Money/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devere/Principles_of_Finance_with_Excel/Time_value_of_Money/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E35D360-74AC-714B-BB49-80D45B8CC44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9EC54F-01DF-BF46-83ED-F8DA11CA5951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{955A6CFD-25FF-FB49-8774-CA448FD17343}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{955A6CFD-25FF-FB49-8774-CA448FD17343}"/>
   </bookViews>
   <sheets>
     <sheet name="Present Value" sheetId="1" r:id="rId1"/>
+    <sheet name="Present Value with Varying Rate" sheetId="3" r:id="rId2"/>
+    <sheet name="Present Value of Annuity" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Simple Present Value Calculation</t>
   </si>
@@ -44,14 +46,95 @@
     <t>Future Payment (X)</t>
   </si>
   <si>
-    <t>Time of Future Paymenr</t>
+    <t xml:space="preserve">Interest Rate (r) </t>
+  </si>
+  <si>
+    <t>Present Value ((X)/(1+r)^n</t>
+  </si>
+  <si>
+    <t>Payment Value Today</t>
+  </si>
+  <si>
+    <t>Future Value in years</t>
+  </si>
+  <si>
+    <t>Time of Future Payment  in Years(n)</t>
+  </si>
+  <si>
+    <t>Simple Present Value Calculation with Varying Discount Rate</t>
+  </si>
+  <si>
+    <t>Table: How does the discount rate affect the present value?</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>Present Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present Value of an Annuity </t>
+  </si>
+  <si>
+    <t>Annual Payment, X</t>
+  </si>
+  <si>
+    <t>Interest Rate (discount rate), r</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Present value of Payment</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Payment at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">end </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of year</t>
+    </r>
+  </si>
+  <si>
+    <t>Present Value of All Payments</t>
+  </si>
+  <si>
+    <t>Summing the Present Values</t>
+  </si>
+  <si>
+    <t>Excel's PV Function</t>
+  </si>
+  <si>
+    <t>Excel's NPV Function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,6 +145,28 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -87,9 +192,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -426,33 +564,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D802DB-AF9B-5E48-9F0D-2A861C421840}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.27E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B2/(1+B4)^B3</f>
+        <v>90.798248057704029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <f>B5</f>
+        <v>90.798248057704029</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B7*(1+B4)^B3</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -461,4 +641,450 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5144588D-9111-C940-9DFD-E48CDE289682}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.27E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B2/(1+B4)^B3</f>
+        <v>90.798248057704029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <f>B5</f>
+        <v>90.798248057704029</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <f>B7*(1+B4)^B3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <f>$B$2/(1+A12)^$B$3</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f>A12+1%</f>
+        <v>0.01</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" ref="B13:B30" si="0">$B$2/(1+A13)^$B$3</f>
+        <v>97.059014792764458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" ref="A14:A21" si="1">A13+1%</f>
+        <v>0.02</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>94.232233454704456</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>91.514165935315958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>88.899635867091476</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>86.383759853147595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>83.961928303230167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>81.629787689085191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f>A19+1%</f>
+        <v>0.08</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>79.383224102016953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>77.21834800610641</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f>A21+1%</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>75.131480090157751</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f>A22+5%</f>
+        <v>0.15</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>65.751623243198836</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" ref="A24:A30" si="2">A23+5%</f>
+        <v>0.2</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>57.870370370370374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>45.516613563950834</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>40.64421074023268</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="2"/>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>36.443148688046655</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="2"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
+        <v>32.801672885317153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="2"/>
+        <v>0.49999999999999994</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
+        <v>29.62962962962963</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A10:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F45C12-2DB1-9048-80C8-EEEA804ABCC2}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="22" style="11" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <f>$B$2</f>
+        <v>100</v>
+      </c>
+      <c r="C6" s="2">
+        <f>$B$2/(1+$B$3)^A6</f>
+        <v>94.339622641509436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <f>A6+1</f>
+        <v>2</v>
+      </c>
+      <c r="B7" s="13">
+        <f t="shared" ref="B7:B10" si="0">$B$2</f>
+        <v>100</v>
+      </c>
+      <c r="C7" s="2">
+        <f>$B$2/(1+$B$3)^A7</f>
+        <v>88.999644001423988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <f t="shared" ref="A8:A10" si="1">A7+1</f>
+        <v>3</v>
+      </c>
+      <c r="B8" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C10" si="2">$B$2/(1+$B$3)^A8</f>
+        <v>83.961928303230167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B9" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="2"/>
+        <v>79.209366323802044</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="2"/>
+        <v>74.72581728660569</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="13">
+        <f>SUM(C6:C10)</f>
+        <v>421.23637855657137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="16">
+        <f>PV($B$3,$A$10,-$B$2)</f>
+        <v>421.23637855657182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="16">
+        <f>NPV($B$3,B6:B10)</f>
+        <v>421.23637855657137</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Present Value Excel sheet
</commit_message>
<xml_diff>
--- a/Time_value_of_Money/Present_Value.xlsx
+++ b/Time_value_of_Money/Present_Value.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devere/Principles_of_Finance_with_Excel/Time_value_of_Money/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9EC54F-01DF-BF46-83ED-F8DA11CA5951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31BF5AF-1DB8-E343-A37E-23A37D7315D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{955A6CFD-25FF-FB49-8774-CA448FD17343}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{955A6CFD-25FF-FB49-8774-CA448FD17343}"/>
   </bookViews>
   <sheets>
     <sheet name="Present Value" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Simple Present Value Calculation</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Excel's NPV Function</t>
+  </si>
+  <si>
+    <t>Present Value, (X)/(1+r)^n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest Rate, r </t>
+  </si>
+  <si>
+    <t>Time of Future Payment  in Years, n</t>
+  </si>
+  <si>
+    <t>Future Payment, X</t>
   </si>
 </sst>
 </file>
@@ -647,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5144588D-9111-C940-9DFD-E48CDE289682}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -667,7 +679,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
         <v>100</v>
@@ -675,7 +687,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -683,7 +695,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3">
         <v>3.27E-2</v>
@@ -691,7 +703,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2">
         <f>B2/(1+B4)^B3</f>
@@ -933,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F45C12-2DB1-9048-80C8-EEEA804ABCC2}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>